<commit_message>
Primeiro commit - adicionando automação RPA
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lc82007\Documents\UiPath\Observabilidade_001_AgentZabbix\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B240CA4-079B-478E-B413-4564BDEDF8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C098B9-CC46-4854-8A94-EB50CC80FE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4215" yWindow="2235" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -219,10 +219,10 @@
     <t>sc start "Zabbix Agent"</t>
   </si>
   <si>
-    <t>C:\Users\[Usuario]\Saque e Pague\Saque e Pague - Zabbix ATM - 5 - BR</t>
-  </si>
-  <si>
     <t>rpa@saqueepague.com.br</t>
+  </si>
+  <si>
+    <t>C:\Users\[usuario]\Documents\Tz0\Tnet Zabbix</t>
   </si>
 </sst>
 </file>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -758,7 +758,7 @@
         <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
@@ -767,7 +767,7 @@
         <v>59</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>